<commit_message>
export excel works, need some tuning on rendering
</commit_message>
<xml_diff>
--- a/data/inscriptions-cantine/2023-10-01.xlsx
+++ b/data/inscriptions-cantine/2023-10-01.xlsx
@@ -393,7 +393,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,6 +473,62 @@
       </c>
       <c r="G4" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>